<commit_message>
Deploying to gh-pages from  @ b1deccb01b972a0f13068876ec93a0e38c3bce89 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.2.1.1a.xlsx
+++ b/en/downloads/data-excel/1.2.1.1a.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="112">
   <si>
     <t>Көрсөткүчтөрдүн аталышы</t>
   </si>
@@ -570,7 +570,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -674,6 +674,12 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -8426,10 +8432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8440,7 +8446,7 @@
     <col min="4" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -8455,7 +8461,7 @@
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -8470,7 +8476,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
@@ -8479,7 +8485,7 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -8507,8 +8513,11 @@
       <c r="I4" s="8">
         <v>2020</v>
       </c>
+      <c r="J4" s="8">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>87</v>
       </c>
@@ -8536,8 +8545,11 @@
       <c r="I5" s="38">
         <v>17.2</v>
       </c>
+      <c r="J5" s="41">
+        <v>24.7</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>95</v>
       </c>
@@ -8553,8 +8565,9 @@
       <c r="G6" s="17"/>
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
+      <c r="J6" s="42"/>
     </row>
-    <row r="7" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>97</v>
       </c>
@@ -8582,8 +8595,11 @@
       <c r="I7" s="14">
         <v>18.7</v>
       </c>
+      <c r="J7" s="14">
+        <v>26.3</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>98</v>
       </c>
@@ -8611,8 +8627,11 @@
       <c r="I8" s="35">
         <v>14.9</v>
       </c>
+      <c r="J8" s="15">
+        <v>22</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>93</v>
       </c>
@@ -8628,8 +8647,9 @@
       <c r="G9" s="17"/>
       <c r="H9" s="36"/>
       <c r="I9" s="36"/>
+      <c r="J9" s="43"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>6</v>
       </c>
@@ -8657,8 +8677,11 @@
       <c r="I10" s="31">
         <v>11.4</v>
       </c>
+      <c r="J10" s="31">
+        <v>18</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>7</v>
       </c>
@@ -8686,8 +8709,11 @@
       <c r="I11" s="31">
         <v>8.9</v>
       </c>
+      <c r="J11" s="31">
+        <v>17.2</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>8</v>
       </c>
@@ -8715,8 +8741,11 @@
       <c r="I12" s="22">
         <v>15.3</v>
       </c>
+      <c r="J12" s="22">
+        <v>23.2</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
@@ -8744,8 +8773,11 @@
       <c r="I13" s="22">
         <v>22.1</v>
       </c>
+      <c r="J13" s="22">
+        <v>29.1</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>10</v>
       </c>
@@ -8773,8 +8805,11 @@
       <c r="I14" s="22">
         <v>27.5</v>
       </c>
+      <c r="J14" s="22">
+        <v>34.200000000000003</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>11</v>
       </c>
@@ -8802,8 +8837,11 @@
       <c r="I15" s="22">
         <v>25.2</v>
       </c>
+      <c r="J15" s="22">
+        <v>33.4</v>
+      </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>12</v>
       </c>
@@ -8831,8 +8869,11 @@
       <c r="I16" s="22">
         <v>16.100000000000001</v>
       </c>
+      <c r="J16" s="22">
+        <v>26.4</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>13</v>
       </c>
@@ -8860,8 +8901,11 @@
       <c r="I17" s="22">
         <v>12.3</v>
       </c>
+      <c r="J17" s="22">
+        <v>20.100000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>14</v>
       </c>
@@ -8889,8 +8933,11 @@
       <c r="I18" s="22">
         <v>8.9</v>
       </c>
+      <c r="J18" s="22">
+        <v>13</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>15</v>
       </c>
@@ -8918,8 +8965,11 @@
       <c r="I19" s="22">
         <v>10.199999999999999</v>
       </c>
+      <c r="J19" s="22">
+        <v>14.3</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>16</v>
       </c>
@@ -8947,8 +8997,11 @@
       <c r="I20" s="22">
         <v>9.4</v>
       </c>
+      <c r="J20" s="22">
+        <v>17.100000000000001</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>17</v>
       </c>
@@ -8976,8 +9029,11 @@
       <c r="I21" s="22">
         <v>5.0999999999999996</v>
       </c>
+      <c r="J21" s="22">
+        <v>13.6</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>102</v>
       </c>
@@ -8993,8 +9049,9 @@
       <c r="G22" s="22"/>
       <c r="H22" s="34"/>
       <c r="I22" s="34"/>
+      <c r="J22" s="42"/>
     </row>
-    <row r="23" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>106</v>
       </c>
@@ -9022,8 +9079,11 @@
       <c r="I23" s="32">
         <v>12.4</v>
       </c>
+      <c r="J23" s="14">
+        <v>24.8</v>
+      </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>109</v>
       </c>
@@ -9051,8 +9111,11 @@
       <c r="I24" s="32">
         <v>20.100000000000001</v>
       </c>
+      <c r="J24" s="15">
+        <v>24.6</v>
+      </c>
     </row>
-    <row r="25" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>104</v>
       </c>
@@ -9068,8 +9131,9 @@
       <c r="G25" s="17"/>
       <c r="H25" s="36"/>
       <c r="I25" s="36"/>
+      <c r="J25" s="43"/>
     </row>
-    <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>66</v>
       </c>
@@ -9097,8 +9161,11 @@
       <c r="I26" s="32">
         <v>21.1</v>
       </c>
+      <c r="J26" s="32">
+        <v>24.3</v>
+      </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>67</v>
       </c>
@@ -9126,8 +9193,11 @@
       <c r="I27" s="32">
         <v>40.1</v>
       </c>
+      <c r="J27" s="32">
+        <v>47.1</v>
+      </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>68</v>
       </c>
@@ -9155,8 +9225,11 @@
       <c r="I28" s="32">
         <v>13.5</v>
       </c>
+      <c r="J28" s="32">
+        <v>23.6</v>
+      </c>
     </row>
-    <row r="29" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>69</v>
       </c>
@@ -9184,8 +9257,11 @@
       <c r="I29" s="32">
         <v>18.7</v>
       </c>
+      <c r="J29" s="32">
+        <v>28.8</v>
+      </c>
     </row>
-    <row r="30" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>70</v>
       </c>
@@ -9213,8 +9289,11 @@
       <c r="I30" s="32">
         <v>24.4</v>
       </c>
+      <c r="J30" s="32">
+        <v>27.8</v>
+      </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
         <v>71</v>
       </c>
@@ -9242,8 +9321,11 @@
       <c r="I31" s="32">
         <v>21.6</v>
       </c>
+      <c r="J31" s="32">
+        <v>29.9</v>
+      </c>
     </row>
-    <row r="32" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>72</v>
       </c>
@@ -9271,8 +9353,11 @@
       <c r="I32" s="32">
         <v>10.1</v>
       </c>
+      <c r="J32" s="32">
+        <v>20.7</v>
+      </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
         <v>73</v>
       </c>
@@ -9300,8 +9385,11 @@
       <c r="I33" s="32">
         <v>19.399999999999999</v>
       </c>
+      <c r="J33" s="32">
+        <v>26.2</v>
+      </c>
     </row>
-    <row r="34" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>74</v>
       </c>
@@ -9329,8 +9417,11 @@
       <c r="I34" s="32">
         <v>11.6</v>
       </c>
+      <c r="J34" s="32">
+        <v>19.100000000000001</v>
+      </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>75</v>
       </c>
@@ -9358,8 +9449,11 @@
       <c r="I35" s="32">
         <v>5.3</v>
       </c>
+      <c r="J35" s="32">
+        <v>10.7</v>
+      </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>76</v>
       </c>
@@ -9387,8 +9481,11 @@
       <c r="I36" s="32">
         <v>20.5</v>
       </c>
+      <c r="J36" s="32">
+        <v>28.9</v>
+      </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
         <v>77</v>
       </c>
@@ -9412,8 +9509,11 @@
       <c r="I37" s="40">
         <v>9</v>
       </c>
+      <c r="J37" s="32">
+        <v>22.7</v>
+      </c>
     </row>
-    <row r="38" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>78</v>
       </c>
@@ -9441,8 +9541,11 @@
       <c r="I38" s="32">
         <v>21</v>
       </c>
+      <c r="J38" s="32">
+        <v>17.899999999999999</v>
+      </c>
     </row>
-    <row r="39" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>79</v>
       </c>
@@ -9470,8 +9573,11 @@
       <c r="I39" s="32">
         <v>12</v>
       </c>
+      <c r="J39" s="32">
+        <v>24.9</v>
+      </c>
     </row>
-    <row r="40" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>80</v>
       </c>
@@ -9499,8 +9605,11 @@
       <c r="I40" s="32">
         <v>13.1</v>
       </c>
+      <c r="J40" s="32">
+        <v>19.899999999999999</v>
+      </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>81</v>
       </c>
@@ -9528,8 +9637,11 @@
       <c r="I41" s="32">
         <v>22</v>
       </c>
+      <c r="J41" s="32">
+        <v>30.7</v>
+      </c>
     </row>
-    <row r="42" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>82</v>
       </c>
@@ -9557,8 +9669,11 @@
       <c r="I42" s="32">
         <v>22.9</v>
       </c>
+      <c r="J42" s="32">
+        <v>25.1</v>
+      </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>83</v>
       </c>
@@ -9586,8 +9701,11 @@
       <c r="I43" s="32">
         <v>12.6</v>
       </c>
+      <c r="J43" s="32">
+        <v>16.3</v>
+      </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>84</v>
       </c>
@@ -9615,8 +9733,11 @@
       <c r="I44" s="32">
         <v>12.5</v>
       </c>
+      <c r="J44" s="32">
+        <v>24.3</v>
+      </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>85</v>
       </c>
@@ -9644,8 +9765,11 @@
       <c r="I45" s="32">
         <v>36</v>
       </c>
+      <c r="J45" s="32">
+        <v>20.6</v>
+      </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="26" t="s">
         <v>86</v>
       </c>
@@ -9673,8 +9797,11 @@
       <c r="I46" s="28">
         <v>10.7</v>
       </c>
+      <c r="J46" s="44" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>

</xml_diff>